<commit_message>
add update evidence A1-A20 Stage-1 & Stage-2
</commit_message>
<xml_diff>
--- a/FridaBy/evidence.xlsx
+++ b/FridaBy/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605" firstSheet="11" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>kalinin0012</t>
   </si>
   <si>
-    <t>3F60EC1FF63853352FD1F111749F31A940657FD403630F7A2580B14B8EBD60183F60EC1FF63853352FD1F111749F31A940657FD403630F7A2580B14B8EBD6018</t>
-  </si>
-  <si>
     <t>gon-irishub-1</t>
   </si>
   <si>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>5BF760E961818872DC5C58262D1CE63F7F317D8D7E1179F3E3B4B3C936058A9E</t>
+  </si>
+  <si>
+    <t>3F60EC1FF63853352FD1F111749F31A940657FD403630F7A2580B14B8EBD6018</t>
   </si>
 </sst>
 </file>
@@ -942,6 +942,68 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
@@ -962,15 +1024,201 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>24</v>
@@ -978,7 +1226,69 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -986,23 +1296,23 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1010,6 +1320,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
     <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -1024,15 +1372,93 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>78</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
@@ -1040,457 +1466,31 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
@@ -1916,7 +1916,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>